<commit_message>
3DI data update, increasing modularity & performance, correlation analysis
</commit_message>
<xml_diff>
--- a/data/postprocessed/table/MPentropy/kendall/correaltions.xlsx
+++ b/data/postprocessed/table/MPentropy/kendall/correaltions.xlsx
@@ -480,61 +480,61 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>-0.2799475832522333</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1165049664272561</v>
+        <v>0.2090321810254712</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1165049664272561</v>
+        <v>-0.118148624057875</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2829406327519076</v>
+        <v>-0.05271246304120579</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
-        <v>-0.04836508334066744</v>
+        <v>-0.04489725391781101</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.02418254167033372</v>
+        <v>0.170632811130217</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.1861251637762357</v>
+        <v>-0.2492238838232901</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.4689439911324401</v>
+        <v>0.3717155353279262</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1694081056390354</v>
+        <v>0.0660253734085456</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>0.3149196827839555</v>
+        <v>0.0721141320311092</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1450952500220023</v>
+        <v>0.2535374338888151</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.2176428750330035</v>
+        <v>0.2614604786978406</v>
       </c>
       <c r="P2" t="n">
-        <v>0.2829406327519076</v>
+        <v>-0.2199382078615827</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.1930152894482308</v>
+        <v>-0.06485291678922628</v>
       </c>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
-        <v>-0.03802528761961016</v>
+        <v>-0.4227554336590582</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.0641767231677369</v>
+        <v>0.2933123469905549</v>
       </c>
       <c r="U2" t="n">
-        <v>0.1241277020080657</v>
+        <v>0.009921272601481622</v>
       </c>
       <c r="V2" t="n">
-        <v>-0.05554164352432002</v>
+        <v>-0.1610876116140179</v>
       </c>
     </row>
     <row r="3">
@@ -544,61 +544,61 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.009003659529304139</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5438661901184723</v>
+        <v>0.05114354262493992</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5438661901184723</v>
+        <v>0.2703189106102171</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1404581822028611</v>
+        <v>0.6228550295960428</v>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
-        <v>0.8010593708697096</v>
+        <v>0.6752950248477201</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8997412986871715</v>
+        <v>0.1070925184168591</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3238063688368376</v>
+        <v>0.01813576185122696</v>
       </c>
       <c r="J3" t="n">
-        <v>0.01182938010945167</v>
+        <v>0.0003477731161933515</v>
       </c>
       <c r="K3" t="n">
-        <v>0.370042496902512</v>
+        <v>0.5378828208791165</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
-        <v>0.1008609542692491</v>
+        <v>0.5010580359233224</v>
       </c>
       <c r="N3" t="n">
-        <v>0.4496917979688909</v>
+        <v>0.01800535102541572</v>
       </c>
       <c r="O3" t="n">
-        <v>0.2568392579578567</v>
+        <v>0.0147104444533948</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1404581822028611</v>
+        <v>0.04016705954746833</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.3146144552999873</v>
+        <v>0.5378757269451848</v>
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="n">
-        <v>0.8429611815702761</v>
+        <v>8.002855799176172e-05</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5493264095783121</v>
+        <v>1.163841448708466e-06</v>
       </c>
       <c r="U3" t="n">
-        <v>0.246817793124011</v>
+        <v>0.871211386875466</v>
       </c>
       <c r="V3" t="n">
-        <v>0.6043156871777332</v>
+        <v>0.007995765619599986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>